<commit_message>
added new socket message type + response
</commit_message>
<xml_diff>
--- a/doc/backend/responselist.xlsx
+++ b/doc/backend/responselist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\IMU_Tracker\doc\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Nextcloud\02 - Projekte\GitHub\IMU_Tracker\doc\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A326D31-CB18-4C0F-A812-8302C62EA494}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F536328-F0D1-4448-B063-4CDC1E22BA75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34605" yWindow="0" windowWidth="16995" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10365" yWindow="2370" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
   <si>
     <t>Options</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>UNKNOWN ERROR</t>
+  </si>
+  <si>
+    <t>DEVICE LOGGOUT FAILED</t>
+  </si>
+  <si>
+    <t>DEVICE LOGGED OUT</t>
   </si>
 </sst>
 </file>
@@ -488,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,6 +604,9 @@
       <c r="B12" s="1">
         <v>8</v>
       </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>5</v>
       </c>
@@ -605,6 +614,9 @@
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
implemented login, logout, new database structure, updated debug website
</commit_message>
<xml_diff>
--- a/doc/backend/responselist.xlsx
+++ b/doc/backend/responselist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Nextcloud\02 - Projekte\GitHub\IMU_Tracker\doc\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F536328-F0D1-4448-B063-4CDC1E22BA75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455BE6C1-FD76-4838-8534-AA1638BCFA47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10365" yWindow="2370" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26310" yWindow="240" windowWidth="17130" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changed observer message to subscriber message
</commit_message>
<xml_diff>
--- a/doc/backend/responselist.xlsx
+++ b/doc/backend/responselist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Nextcloud\02 - Projekte\GitHub\IMU_Tracker\doc\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455BE6C1-FD76-4838-8534-AA1638BCFA47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5801ABA5-7125-4D9F-86CD-582A3E4429A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26310" yWindow="240" windowWidth="17130" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -66,12 +66,6 @@
     <t>DEVICE REGISTERED</t>
   </si>
   <si>
-    <t>OBSERVER REGISTERED</t>
-  </si>
-  <si>
-    <t>OBSERVER UNREGISTERED</t>
-  </si>
-  <si>
     <t>MISSING API KEY</t>
   </si>
   <si>
@@ -87,24 +81,9 @@
     <t>INVALID DEVICE ID</t>
   </si>
   <si>
-    <t>OBSERVER ALREADY REGISTERED</t>
-  </si>
-  <si>
-    <t>OBSERVER NOT REGISTERED</t>
-  </si>
-  <si>
     <t>MISSING DEVICE ID</t>
   </si>
   <si>
-    <t>OBSERVER MISSING REGESTRATION STATE</t>
-  </si>
-  <si>
-    <t>OBSERVER CANT REGISTER AS DEVICE</t>
-  </si>
-  <si>
-    <t>DEVICE CANT REGISTER AS OBSERVER</t>
-  </si>
-  <si>
     <t>MISSING TYPE</t>
   </si>
   <si>
@@ -124,6 +103,27 @@
   </si>
   <si>
     <t>DEVICE LOGGED OUT</t>
+  </si>
+  <si>
+    <t>SUBSCRIBER REGISTERED</t>
+  </si>
+  <si>
+    <t>SUBSCRIBER UNREGISTERED</t>
+  </si>
+  <si>
+    <t>SUBSCRIBER ALREADY REGISTERED</t>
+  </si>
+  <si>
+    <t>SUBSCRIBER NOT REGISTERED</t>
+  </si>
+  <si>
+    <t>SUBSCRIBER MISSING REGESTRATION STATE</t>
+  </si>
+  <si>
+    <t>SUBSCRIBER CANT REGISTER AS DEVICE</t>
+  </si>
+  <si>
+    <t>DEVICE CANT REGISTER AS SUBSCRIBER</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -605,7 +605,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>5</v>
@@ -616,7 +616,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>5</v>
@@ -638,7 +638,7 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>4</v>
@@ -649,7 +649,7 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>5</v>
@@ -708,7 +708,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>4</v>
@@ -719,7 +719,7 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>4</v>
@@ -730,7 +730,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>4</v>
@@ -741,7 +741,7 @@
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>5</v>
@@ -752,7 +752,7 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D27" s="1" t="str">
         <f>IF(ISBLANK(C27),$I$4,$I$5)</f>
@@ -764,7 +764,7 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D28" s="1" t="str">
         <f>IF(ISBLANK(C28),$I$4,$I$5)</f>
@@ -776,7 +776,7 @@
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>5</v>
@@ -787,7 +787,7 @@
         <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D30" s="1" t="str">
         <f>IF(ISBLANK(C30),$I$4,$I$5)</f>
@@ -799,7 +799,7 @@
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D31" s="1" t="str">
         <f>IF(ISBLANK(C31),$I$4,$I$5)</f>
@@ -811,7 +811,7 @@
         <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>5</v>
@@ -822,7 +822,7 @@
         <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>5</v>
@@ -833,7 +833,7 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D34" s="1" t="str">
         <f>IF(ISBLANK(C34),$I$4,$I$5)</f>
@@ -845,7 +845,7 @@
         <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>5</v>
@@ -856,7 +856,7 @@
         <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D36" s="1" t="str">
         <f>IF(ISBLANK(C36),$I$4,$I$5)</f>
@@ -924,7 +924,7 @@
         <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>5</v>
@@ -943,7 +943,7 @@
         <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>5</v>

</xml_diff>